<commit_message>
01/06/2025 23:33:22 LAPTOP-NDBD612Q commit
</commit_message>
<xml_diff>
--- a/raw/test_kalimat.xlsx
+++ b/raw/test_kalimat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adi\Downloads\Project-NLP\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90DFC4A-57A8-429D-994B-B2C384243B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1040F877-4B66-4912-991B-A7ED7E542DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Sentence</t>
   </si>
@@ -121,24 +121,12 @@
     <t xml:space="preserve">Ada pandita ajaka duang diri </t>
   </si>
   <si>
-    <t xml:space="preserve">Luh cang sing I Donglen </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tan sipi pakrepekane I Lutung </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keto pawuwus Ida Batara Indra </t>
-  </si>
-  <si>
     <t xml:space="preserve">Siput ane malunan masaut </t>
   </si>
   <si>
     <t xml:space="preserve">Nyen adan caine Gede </t>
   </si>
   <si>
-    <t xml:space="preserve">Ngaduh-ngaduh I Klaleng ngorang sakit </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ditu ia mabakti sambila ngacep </t>
   </si>
   <si>
@@ -151,54 +139,21 @@
     <t xml:space="preserve">Tiang naur nika </t>
   </si>
   <si>
-    <t xml:space="preserve">Sinah pungkuran bakal nemu bagia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I Lutung lantas ngomong </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kacerita ada alu gede gati </t>
-  </si>
-  <si>
     <t xml:space="preserve">Keto munyin memene </t>
   </si>
   <si>
     <t xml:space="preserve">Keto bikas alune totonan </t>
   </si>
   <si>
-    <t xml:space="preserve">Ia nyambatang awakne genit kaukud </t>
-  </si>
-  <si>
     <t xml:space="preserve">Masaut bin curike ne muani </t>
   </si>
   <si>
-    <t xml:space="preserve">Masih ajahina I Ubuh masastra </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sajaan ento Dong </t>
   </si>
   <si>
-    <t xml:space="preserve">Mailehan alih-alihina masih tusing tepukina </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kadung i dewek ngelah daya </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sang Nandaka ngelarang kapanditan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keto abetne I Lutung </t>
-  </si>
-  <si>
     <t xml:space="preserve">Inggih titiang sairing </t>
   </si>
   <si>
-    <t xml:space="preserve">Makejang wong purine ledang pisan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I Kepuh nombahang </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ratun kedise uli delod pasih </t>
   </si>
   <si>
@@ -299,6 +254,48 @@
   </si>
   <si>
     <t>(K (S (NP (Noun dadong))) (P (VP (Adv suba) (VP (Verb batara)))) (Pel (NP (Noun sri))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Noun ada))) (P (NP (Noun pandita))) (Ket (PP (Prep ajaka) (NP (NP (Noun duang)) (Noun diri)))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Noun siput))) (P (PP (Prep ane) (NP (NP (Noun malunan)) (Pronoun masaut)))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Noun nyen))) (P (NP (Noun adan))) (Pel (NP (NP (Pronoun caine)) (Adj gede))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Pronoun ditu))) (P (NP (NP (Pronoun ia)) (Noun mabakti))) (Pel (NP (NP (Noun sambila)) (Noun ngacep))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Noun dadinne))) (P (NP (NP (Noun suung)) (Pronoun ditu))) (Pel (NP (NP (Noun kubune)) (Pronoun ento))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Noun ada))) (P (NP (Pronoun anake))) (Pel (NP (NP (Pronoun ngeling)) (Noun mapangenan))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Pronoun tiang))) (P (NP (NP (Noun naur)) (Pronoun nika))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Noun keto))) (P (NP (NP (Noun munyin)) (Pronoun memene))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Noun keto))) (P (VP (Verb bikas))) (Pel (NP (NP (Noun alune)) (Pronoun totonan))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Pronoun masaut))) (P (NP (NP (Noun bin)) (Noun curike))) (Pel (NP (NP (Pronoun ne)) (Noun muani))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Noun sajaan))) (P (NP (NP (Pronoun ento)) (Pronoun dong))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Noun inggih))) (P (NP (NP (Pronoun titiang)) (Noun sairing))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Pronoun mataluh))) (P (NP (NP (Noun sabilang)) (Noun wai))))</t>
+  </si>
+  <si>
+    <t>(K (S (NP (Noun ratun))) (P (NP (Pronoun kedise))) (Ket (PP (Prep uli) (NP (NP (Noun delod)) (Noun pasih)))))</t>
   </si>
 </sst>
 </file>
@@ -670,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -695,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -703,7 +700,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,7 +708,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -719,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -727,7 +724,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -735,7 +732,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -743,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -751,7 +748,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -759,7 +756,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -767,7 +764,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -775,7 +772,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -783,7 +780,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -791,7 +788,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -799,7 +796,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -807,7 +804,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -815,7 +812,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -823,7 +820,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -831,7 +828,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -839,7 +836,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -847,7 +844,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -855,7 +852,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -863,7 +860,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -871,7 +868,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -879,7 +876,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -887,7 +884,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -895,7 +892,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -903,7 +900,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -911,7 +908,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -919,7 +916,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -927,7 +924,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -935,152 +932,119 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>60</v>
+      <c r="B46" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>